<commit_message>
LE0703, LE1001: Escaletas ajustadas
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion03/Escaleta_LE_07_03_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion03/Escaleta_LE_07_03_CO.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$39</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1458,22 +1458,13 @@
     <xf numFmtId="0" fontId="8" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1498,6 +1489,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1994,8 +1994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3:P38"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -2023,94 +2023,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.85" x14ac:dyDescent="0.45">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="48"/>
-      <c r="O1" s="36" t="s">
+      <c r="N1" s="45"/>
+      <c r="O1" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="T1" s="38" t="s">
+      <c r="T1" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="U1" s="47" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.85" x14ac:dyDescent="0.45">
-      <c r="A2" s="43"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="44"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="41"/>
       <c r="M2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="37"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="47"/>
     </row>
     <row r="3" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A3" s="6" t="s">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="M3" s="15"/>
       <c r="N3" s="16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O3" s="17" t="s">
         <v>232</v>
@@ -4328,6 +4328,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4342,12 +4348,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I32:I39 I28:I30 I23:I26 I18:I21 I15:I16 I13 I3:I8 I10">

</xml_diff>

<commit_message>
Actualización de escaleta guion 3 de 7
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion03/Escaleta_LE_07_03_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion03/Escaleta_LE_07_03_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Documents\GitHub\Lenguaje\fuentes\contenidos\grado07\guion03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csepulveda\Desktop\GITHUB2015\Lenguaje\fuentes\contenidos\grado07\guion03\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -368,12 +368,6 @@
     <t>Recurso M13A-01</t>
   </si>
   <si>
-    <t>Lee el texto y corrige las palabras mal escritas</t>
-  </si>
-  <si>
-    <t>Actividad para diagnosticar el uso correcto de las palabras terminadas en -sión y -ción</t>
-  </si>
-  <si>
     <t>Recurso M12B-01</t>
   </si>
   <si>
@@ -407,9 +401,6 @@
     <t>Recurso M5C-01</t>
   </si>
   <si>
-    <t>Escucha atentamente el haikú o el tanka y responde las preguntas</t>
-  </si>
-  <si>
     <t>Actividad con audio sobre las composiciones líricas de origen japonés</t>
   </si>
   <si>
@@ -470,9 +461,6 @@
     <t>Recurso F6B-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Literatura: las composiciones líricas breves </t>
-  </si>
-  <si>
     <t>Recurso M101A-02</t>
   </si>
   <si>
@@ -560,12 +548,6 @@
     <t>Actividad para diferenciar diferentes complementos verbales</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Gramática: los complementos verbales atributo, directo e indirecto </t>
-  </si>
-  <si>
-    <t>Actividad para profundizar la comprensión de los complementos verbales atributo, directo e indirecto</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ortografía: las palabras terminadas en -sión y -ción </t>
   </si>
   <si>
@@ -605,21 +587,12 @@
     <t>Recurso M101A-03</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Ortografía: las palabras terminadas en -sión y -ción</t>
-  </si>
-  <si>
     <t>Recurso M101A-04</t>
   </si>
   <si>
     <t>Recurso M2C-01</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: selecciona en el texto la palabra bien escrita</t>
-  </si>
-  <si>
-    <t>Actividad para investigar sobre el origen y la función de los sufijos -ción y el -sión</t>
-  </si>
-  <si>
     <t xml:space="preserve">Actividad para afianzar la ortografía de palabras con los sufijos -ción y -sión </t>
   </si>
   <si>
@@ -641,18 +614,12 @@
     <t>Escucha la biografía y organiza los sucesos cronológicamente</t>
   </si>
   <si>
-    <t>Actividad para poner en práctica el establecer la cronología de una biografía</t>
-  </si>
-  <si>
     <t>Recurso M3B1-01</t>
   </si>
   <si>
     <t>Actividad diagnóstica con audios de comprensión sobre la biografía</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Comprensión textual: la biografía </t>
-  </si>
-  <si>
     <t>Recurso M101A-05</t>
   </si>
   <si>
@@ -698,9 +665,6 @@
     <t>Recurso F10B-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Producción escrita: la biografía  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Actividad para redactar una autobiografía y afianzar los conocimientos sobre el texto biográfico </t>
   </si>
   <si>
@@ -717,9 +681,6 @@
   </si>
   <si>
     <t>Crucigrama de datos biográficos</t>
-  </si>
-  <si>
-    <t>Actividad lúdica sobre la vida de un célebre escritor</t>
   </si>
   <si>
     <t xml:space="preserve">Diseñar un crucigrama con datos biográficos de un escritor. Por ejemplo: "Cien: Primera palabra de su novela más célebre; Aura: nombre de su esposa, etc." </t>
@@ -875,12 +836,70 @@
   <si>
     <t>(DBA: 12,10) Proponer un ejemplo de cada uno de los géneros de la sección para que el estudiante lo asocie con la etiqueta correspondiente: haikú, tanka, epigrama, caligrama y greguería. Si el caligrama se ponde difícil, sumprimirlo, pero en lo posible que esté incluído.</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lee el texto y corrige las palabras escritas de forma incorrecta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Actividad para practicar el uso correcto de las palabras terminadas en -sión y -ción</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escucha atentamente el haikú y el tanka </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: Las composiciones líricas breves </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: Los complementos verbales atributo, directo e indirecto </t>
+  </si>
+  <si>
+    <t>Actividad para profundizar en la comprensión de los complementos verbales atributo, directo e indirecto</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Las palabras terminadas en -sión y -ción</t>
+  </si>
+  <si>
+    <t>Actividad para investigar sobre el origen y la función de los sufijos -ción y -sión</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: selecciona en el texto la palabra escrita correctamente</t>
+  </si>
+  <si>
+    <t>Actividad para identificar el orden de los hechos en una biografía</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: La biografía </t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: redacta tu autobiografía</t>
+  </si>
+  <si>
+    <t>Actividad lúdica sobre la vida de un escritor célebre</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -945,6 +964,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1359,7 +1385,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1458,22 +1484,13 @@
     <xf numFmtId="0" fontId="8" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1499,6 +1516,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="189">
@@ -1994,8 +2029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" topLeftCell="G20" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2022,94 +2057,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="48"/>
-      <c r="O1" s="36" t="s">
+      <c r="N1" s="45"/>
+      <c r="O1" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="T1" s="38" t="s">
+      <c r="T1" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="U1" s="47" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="44"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="41"/>
       <c r="M2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="37"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="47"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2149,7 +2184,7 @@
         <v>36</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="P3" s="18" t="s">
         <v>19</v>
@@ -2208,7 +2243,7 @@
         <v>23</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="P4" s="25" t="s">
         <v>19</v>
@@ -2267,7 +2302,7 @@
         <v>26</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="P5" s="25" t="s">
         <v>19</v>
@@ -2304,7 +2339,7 @@
       <c r="E6" s="22"/>
       <c r="F6" s="23"/>
       <c r="G6" s="11" t="s">
-        <v>101</v>
+        <v>251</v>
       </c>
       <c r="H6" s="10">
         <v>4</v>
@@ -2312,8 +2347,8 @@
       <c r="I6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="12" t="s">
-        <v>102</v>
+      <c r="J6" s="50" t="s">
+        <v>252</v>
       </c>
       <c r="K6" s="13" t="s">
         <v>20</v>
@@ -2326,7 +2361,7 @@
         <v>49</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="P6" s="25" t="s">
         <v>19</v>
@@ -2363,7 +2398,7 @@
       <c r="E7" s="22"/>
       <c r="F7" s="23"/>
       <c r="G7" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="H7" s="10">
         <v>5</v>
@@ -2372,7 +2407,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="K7" s="13" t="s">
         <v>20</v>
@@ -2385,7 +2420,7 @@
         <v>31</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="P7" s="25" t="s">
         <v>19</v>
@@ -2400,7 +2435,7 @@
         <v>89</v>
       </c>
       <c r="T7" s="28" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="U7" s="26" t="s">
         <v>91</v>
@@ -2422,7 +2457,7 @@
       <c r="E8" s="22"/>
       <c r="F8" s="23"/>
       <c r="G8" s="11" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="H8" s="10">
         <v>6</v>
@@ -2431,7 +2466,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>20</v>
@@ -2444,7 +2479,7 @@
         <v>52</v>
       </c>
       <c r="O8" s="17" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="P8" s="25" t="s">
         <v>19</v>
@@ -2459,7 +2494,7 @@
         <v>89</v>
       </c>
       <c r="T8" s="28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U8" s="26" t="s">
         <v>91</v>
@@ -2476,14 +2511,14 @@
         <v>86</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H9" s="10">
         <v>7</v>
@@ -2492,7 +2527,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>20</v>
@@ -2505,7 +2540,7 @@
       </c>
       <c r="N9" s="30"/>
       <c r="O9" s="17" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="P9" s="31" t="s">
         <v>19</v>
@@ -2514,16 +2549,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="S9" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="T9" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="S9" s="26" t="s">
+      <c r="U9" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="T9" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="U9" s="26" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2537,14 +2572,14 @@
         <v>86</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F10" s="23"/>
-      <c r="G10" s="11" t="s">
-        <v>114</v>
+      <c r="G10" s="51" t="s">
+        <v>253</v>
       </c>
       <c r="H10" s="10">
         <v>8</v>
@@ -2553,7 +2588,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K10" s="13" t="s">
         <v>20</v>
@@ -2566,7 +2601,7 @@
         <v>35</v>
       </c>
       <c r="O10" s="17" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="P10" s="25" t="s">
         <v>19</v>
@@ -2581,7 +2616,7 @@
         <v>89</v>
       </c>
       <c r="T10" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="U10" s="19" t="s">
         <v>91</v>
@@ -2598,14 +2633,14 @@
         <v>86</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H11" s="10">
         <v>9</v>
@@ -2614,7 +2649,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K11" s="13" t="s">
         <v>20</v>
@@ -2627,7 +2662,7 @@
         <v>36</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="P11" s="25" t="s">
         <v>19</v>
@@ -2642,7 +2677,7 @@
         <v>89</v>
       </c>
       <c r="T11" s="21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="U11" s="19" t="s">
         <v>91</v>
@@ -2659,14 +2694,14 @@
         <v>86</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H12" s="10">
         <v>10</v>
@@ -2675,7 +2710,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>19</v>
@@ -2686,25 +2721,25 @@
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
       <c r="O12" s="17" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="P12" s="25" t="s">
         <v>19</v>
       </c>
       <c r="Q12" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="R12" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="S12" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="T12" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="U12" s="26" t="s">
         <v>118</v>
-      </c>
-      <c r="R12" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="S12" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="T12" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="U12" s="26" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2718,14 +2753,14 @@
         <v>86</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H13" s="10">
         <v>11</v>
@@ -2734,7 +2769,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="K13" s="13" t="s">
         <v>20</v>
@@ -2747,7 +2782,7 @@
         <v>32</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="P13" s="25" t="s">
         <v>19</v>
@@ -2762,7 +2797,7 @@
         <v>89</v>
       </c>
       <c r="T13" s="21" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="U13" s="19" t="s">
         <v>91</v>
@@ -2779,14 +2814,14 @@
         <v>86</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H14" s="10">
         <v>12</v>
@@ -2795,7 +2830,7 @@
         <v>19</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K14" s="13" t="s">
         <v>20</v>
@@ -2808,7 +2843,7 @@
       </c>
       <c r="N14" s="16"/>
       <c r="O14" s="17" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="P14" s="25" t="s">
         <v>19</v>
@@ -2817,16 +2852,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S14" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="T14" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="U14" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="T14" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="U14" s="26" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2840,14 +2875,14 @@
         <v>86</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F15" s="23"/>
-      <c r="G15" s="11" t="s">
-        <v>135</v>
+      <c r="G15" s="51" t="s">
+        <v>254</v>
       </c>
       <c r="H15" s="10">
         <v>13</v>
@@ -2856,7 +2891,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K15" s="13" t="s">
         <v>20</v>
@@ -2869,7 +2904,7 @@
         <v>52</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="P15" s="25" t="s">
         <v>19</v>
@@ -2884,7 +2919,7 @@
         <v>89</v>
       </c>
       <c r="T15" s="28" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="U15" s="26" t="s">
         <v>91</v>
@@ -2901,14 +2936,14 @@
         <v>86</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H16" s="10">
         <v>14</v>
@@ -2917,7 +2952,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="K16" s="13" t="s">
         <v>20</v>
@@ -2930,7 +2965,7 @@
         <v>23</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="P16" s="25" t="s">
         <v>20</v>
@@ -2945,7 +2980,7 @@
         <v>89</v>
       </c>
       <c r="T16" s="21" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="U16" s="19" t="s">
         <v>91</v>
@@ -2962,14 +2997,14 @@
         <v>86</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H17" s="10">
         <v>15</v>
@@ -2978,7 +3013,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K17" s="13" t="s">
         <v>20</v>
@@ -2991,7 +3026,7 @@
       </c>
       <c r="N17" s="16"/>
       <c r="O17" s="17" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="P17" s="25" t="s">
         <v>19</v>
@@ -3000,16 +3035,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S17" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="T17" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="U17" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="T17" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="U17" s="26" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3023,14 +3058,14 @@
         <v>86</v>
       </c>
       <c r="D18" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="22" t="s">
         <v>145</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>149</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="11" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H18" s="10">
         <v>16</v>
@@ -3039,7 +3074,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K18" s="13" t="s">
         <v>20</v>
@@ -3052,7 +3087,7 @@
         <v>50</v>
       </c>
       <c r="O18" s="23" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="P18" s="25" t="s">
         <v>19</v>
@@ -3067,7 +3102,7 @@
         <v>89</v>
       </c>
       <c r="T18" s="28" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="U18" s="26" t="s">
         <v>91</v>
@@ -3084,14 +3119,14 @@
         <v>86</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H19" s="10">
         <v>17</v>
@@ -3100,7 +3135,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="24" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="K19" s="13" t="s">
         <v>20</v>
@@ -3113,7 +3148,7 @@
         <v>50</v>
       </c>
       <c r="O19" s="23" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="P19" s="25" t="s">
         <v>19</v>
@@ -3128,7 +3163,7 @@
         <v>89</v>
       </c>
       <c r="T19" s="21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="U19" s="19" t="s">
         <v>91</v>
@@ -3145,14 +3180,14 @@
         <v>86</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F20" s="23"/>
       <c r="G20" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H20" s="10">
         <v>18</v>
@@ -3161,7 +3196,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="K20" s="13" t="s">
         <v>20</v>
@@ -3174,7 +3209,7 @@
         <v>50</v>
       </c>
       <c r="O20" s="23" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="P20" s="25" t="s">
         <v>19</v>
@@ -3189,7 +3224,7 @@
         <v>89</v>
       </c>
       <c r="T20" s="21" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="U20" s="19" t="s">
         <v>91</v>
@@ -3206,14 +3241,14 @@
         <v>86</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F21" s="23"/>
-      <c r="G21" s="11" t="s">
-        <v>165</v>
+      <c r="G21" s="51" t="s">
+        <v>255</v>
       </c>
       <c r="H21" s="10">
         <v>19</v>
@@ -3222,7 +3257,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="24" t="s">
-        <v>166</v>
+        <v>256</v>
       </c>
       <c r="K21" s="13" t="s">
         <v>20</v>
@@ -3235,7 +3270,7 @@
         <v>52</v>
       </c>
       <c r="O21" s="23" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="P21" s="25" t="s">
         <v>19</v>
@@ -3250,7 +3285,7 @@
         <v>89</v>
       </c>
       <c r="T21" s="28" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="U21" s="26" t="s">
         <v>91</v>
@@ -3267,14 +3302,14 @@
         <v>86</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F22" s="23"/>
       <c r="G22" s="11" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="H22" s="10">
         <v>20</v>
@@ -3283,7 +3318,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="K22" s="13" t="s">
         <v>20</v>
@@ -3296,7 +3331,7 @@
       </c>
       <c r="N22" s="16"/>
       <c r="O22" s="23" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="P22" s="25" t="s">
         <v>19</v>
@@ -3305,16 +3340,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S22" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="T22" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="U22" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="T22" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="U22" s="26" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3328,14 +3363,14 @@
         <v>86</v>
       </c>
       <c r="D23" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="22" t="s">
         <v>167</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>173</v>
       </c>
       <c r="F23" s="23"/>
       <c r="G23" s="11" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H23" s="10">
         <v>21</v>
@@ -3344,7 +3379,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="24" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="K23" s="13" t="s">
         <v>20</v>
@@ -3357,7 +3392,7 @@
         <v>25</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="P23" s="25" t="s">
         <v>19</v>
@@ -3372,7 +3407,7 @@
         <v>89</v>
       </c>
       <c r="T23" s="21" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="U23" s="19" t="s">
         <v>91</v>
@@ -3389,14 +3424,14 @@
         <v>86</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F24" s="23"/>
       <c r="G24" s="11" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H24" s="10">
         <v>22</v>
@@ -3405,7 +3440,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="K24" s="13" t="s">
         <v>20</v>
@@ -3418,7 +3453,7 @@
         <v>38</v>
       </c>
       <c r="O24" s="23" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="P24" s="25" t="s">
         <v>19</v>
@@ -3433,7 +3468,7 @@
         <v>89</v>
       </c>
       <c r="T24" s="21" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="U24" s="19" t="s">
         <v>91</v>
@@ -3450,14 +3485,14 @@
         <v>86</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F25" s="23"/>
-      <c r="G25" s="11" t="s">
-        <v>180</v>
+      <c r="G25" s="51" t="s">
+        <v>257</v>
       </c>
       <c r="H25" s="10">
         <v>23</v>
@@ -3466,7 +3501,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>184</v>
+        <v>258</v>
       </c>
       <c r="K25" s="13" t="s">
         <v>20</v>
@@ -3479,7 +3514,7 @@
         <v>52</v>
       </c>
       <c r="O25" s="23" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="P25" s="25" t="s">
         <v>19</v>
@@ -3494,7 +3529,7 @@
         <v>89</v>
       </c>
       <c r="T25" s="28" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="U25" s="26" t="s">
         <v>91</v>
@@ -3511,14 +3546,14 @@
         <v>86</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F26" s="23"/>
-      <c r="G26" s="11" t="s">
-        <v>183</v>
+      <c r="G26" s="51" t="s">
+        <v>259</v>
       </c>
       <c r="H26" s="10">
         <v>24</v>
@@ -3527,7 +3562,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="K26" s="13" t="s">
         <v>20</v>
@@ -3540,7 +3575,7 @@
         <v>27</v>
       </c>
       <c r="O26" s="23" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="P26" s="25" t="s">
         <v>20</v>
@@ -3555,7 +3590,7 @@
         <v>89</v>
       </c>
       <c r="T26" s="28" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="U26" s="26" t="s">
         <v>91</v>
@@ -3572,7 +3607,7 @@
         <v>86</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="23"/>
@@ -3586,7 +3621,7 @@
         <v>19</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="K27" s="13" t="s">
         <v>20</v>
@@ -3599,7 +3634,7 @@
       </c>
       <c r="N27" s="16"/>
       <c r="O27" s="17" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="P27" s="25" t="s">
         <v>19</v>
@@ -3608,16 +3643,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S27" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="T27" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="U27" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="T27" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="U27" s="26" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3631,16 +3666,16 @@
         <v>86</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="H28" s="10">
         <v>26</v>
@@ -3648,8 +3683,8 @@
       <c r="I28" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="24" t="s">
-        <v>192</v>
+      <c r="J28" s="50" t="s">
+        <v>260</v>
       </c>
       <c r="K28" s="13" t="s">
         <v>20</v>
@@ -3662,7 +3697,7 @@
         <v>46</v>
       </c>
       <c r="O28" s="17" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="P28" s="25" t="s">
         <v>19</v>
@@ -3677,7 +3712,7 @@
         <v>89</v>
       </c>
       <c r="T28" s="28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="U28" s="26" t="s">
         <v>91</v>
@@ -3694,14 +3729,14 @@
         <v>86</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F29" s="23"/>
-      <c r="G29" s="11" t="s">
-        <v>195</v>
+      <c r="G29" s="51" t="s">
+        <v>261</v>
       </c>
       <c r="H29" s="10">
         <v>27</v>
@@ -3710,7 +3745,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="K29" s="13" t="s">
         <v>20</v>
@@ -3723,7 +3758,7 @@
         <v>52</v>
       </c>
       <c r="O29" s="23" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="P29" s="25" t="s">
         <v>19</v>
@@ -3738,7 +3773,7 @@
         <v>89</v>
       </c>
       <c r="T29" s="28" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="U29" s="26" t="s">
         <v>91</v>
@@ -3755,14 +3790,14 @@
         <v>86</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="F30" s="23"/>
       <c r="G30" s="11" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="H30" s="10">
         <v>28</v>
@@ -3771,7 +3806,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="24" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="K30" s="13" t="s">
         <v>20</v>
@@ -3784,7 +3819,7 @@
         <v>36</v>
       </c>
       <c r="O30" s="23" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="P30" s="25" t="s">
         <v>19</v>
@@ -3799,7 +3834,7 @@
         <v>89</v>
       </c>
       <c r="T30" s="21" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="U30" s="19" t="s">
         <v>91</v>
@@ -3816,14 +3851,14 @@
         <v>86</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="F31" s="23"/>
       <c r="G31" s="11" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="H31" s="10">
         <v>29</v>
@@ -3832,7 +3867,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="24" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K31" s="13" t="s">
         <v>20</v>
@@ -3845,7 +3880,7 @@
       </c>
       <c r="N31" s="16"/>
       <c r="O31" s="23" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="P31" s="25" t="s">
         <v>19</v>
@@ -3854,16 +3889,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S31" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="T31" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="U31" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="T31" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="U31" s="26" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3877,14 +3912,14 @@
         <v>86</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F32" s="23"/>
-      <c r="G32" s="11" t="s">
-        <v>211</v>
+      <c r="G32" s="51" t="s">
+        <v>262</v>
       </c>
       <c r="H32" s="10">
         <v>30</v>
@@ -3893,7 +3928,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="24" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="K32" s="13" t="s">
         <v>20</v>
@@ -3906,7 +3941,7 @@
         <v>52</v>
       </c>
       <c r="O32" s="23" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="P32" s="25" t="s">
         <v>19</v>
@@ -3915,16 +3950,16 @@
         <v>6</v>
       </c>
       <c r="R32" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S32" s="26" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="T32" s="28" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="U32" s="26" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3938,12 +3973,12 @@
         <v>86</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E33" s="22"/>
       <c r="F33" s="23"/>
       <c r="G33" s="11" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H33" s="10">
         <v>31</v>
@@ -3952,7 +3987,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="24" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K33" s="13" t="s">
         <v>20</v>
@@ -3965,7 +4000,7 @@
         <v>84</v>
       </c>
       <c r="O33" s="23" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="P33" s="25" t="s">
         <v>19</v>
@@ -3980,7 +4015,7 @@
         <v>89</v>
       </c>
       <c r="T33" s="28" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="U33" s="26" t="s">
         <v>91</v>
@@ -3997,12 +4032,12 @@
         <v>86</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" s="23"/>
       <c r="G34" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H34" s="10">
         <v>32</v>
@@ -4011,7 +4046,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="24" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="K34" s="13" t="s">
         <v>20</v>
@@ -4024,7 +4059,7 @@
         <v>43</v>
       </c>
       <c r="O34" s="23" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="P34" s="25" t="s">
         <v>19</v>
@@ -4039,7 +4074,7 @@
         <v>89</v>
       </c>
       <c r="T34" s="28" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="U34" s="26" t="s">
         <v>91</v>
@@ -4056,12 +4091,12 @@
         <v>86</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E35" s="22"/>
       <c r="F35" s="23"/>
       <c r="G35" s="11" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="H35" s="10">
         <v>33</v>
@@ -4070,7 +4105,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="24" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="K35" s="13" t="s">
         <v>19</v>
@@ -4081,25 +4116,25 @@
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
       <c r="O35" s="23" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="P35" s="25" t="s">
         <v>19</v>
       </c>
       <c r="Q35" s="26" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="R35" s="27" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="S35" s="26" t="s">
         <v>86</v>
       </c>
       <c r="T35" s="28" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="U35" s="26" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4113,12 +4148,12 @@
         <v>86</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="23"/>
       <c r="G36" s="11" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="H36" s="10">
         <v>34</v>
@@ -4127,7 +4162,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="24" t="s">
-        <v>218</v>
+        <v>263</v>
       </c>
       <c r="K36" s="13" t="s">
         <v>20</v>
@@ -4140,7 +4175,7 @@
         <v>44</v>
       </c>
       <c r="O36" s="23" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="P36" s="25" t="s">
         <v>19</v>
@@ -4155,7 +4190,7 @@
         <v>89</v>
       </c>
       <c r="T36" s="28" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="U36" s="26" t="s">
         <v>91</v>
@@ -4172,7 +4207,7 @@
         <v>86</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" s="23"/>
@@ -4186,7 +4221,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="24" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="K37" s="13" t="s">
         <v>20</v>
@@ -4217,12 +4252,12 @@
         <v>86</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="23"/>
       <c r="G38" s="11" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="H38" s="10">
         <v>36</v>
@@ -4231,7 +4266,7 @@
         <v>20</v>
       </c>
       <c r="J38" s="24" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="K38" s="13" t="s">
         <v>20</v>
@@ -4244,7 +4279,7 @@
         <v>32</v>
       </c>
       <c r="O38" s="23" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="P38" s="25" t="s">
         <v>19</v>
@@ -4259,7 +4294,7 @@
         <v>89</v>
       </c>
       <c r="T38" s="35" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="U38" s="34" t="s">
         <v>91</v>
@@ -4276,7 +4311,7 @@
         <v>86</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="23"/>
@@ -4288,7 +4323,7 @@
         <v>20</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="K39" s="13" t="s">
         <v>20</v>
@@ -4301,7 +4336,7 @@
         <v>53</v>
       </c>
       <c r="O39" s="23" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="P39" s="25" t="s">
         <v>20</v>
@@ -4316,7 +4351,7 @@
         <v>89</v>
       </c>
       <c r="T39" s="28" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="U39" s="26" t="s">
         <v>91</v>
@@ -4327,6 +4362,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4341,12 +4382,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I32:I39 I28:I30 I23:I26 I18:I21 I15:I16 I13 I3:I8 I10">
@@ -4354,7 +4389,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">

</xml_diff>